<commit_message>
Amak2 runs for EBS pollock
</commit_message>
<xml_diff>
--- a/SAM/ebspoll/data/SAM_data_ebswp.xlsx
+++ b/SAM/ebspoll/data/SAM_data_ebswp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/_mymods/afsc-assessments/ebs_pollock_mod_alts/SAM/ebspoll/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B422B5AA-8D6F-574D-8436-FEE323E462C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6837A885-A9B7-7045-B08A-A33C406E23FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-21100" windowWidth="21600" windowHeight="37900" activeTab="10" xr2:uid="{DF91BBF4-075E-1249-A59B-F8187EDF0F86}"/>
+    <workbookView xWindow="4660" yWindow="760" windowWidth="21600" windowHeight="21580" activeTab="5" xr2:uid="{DF91BBF4-075E-1249-A59B-F8187EDF0F86}"/>
   </bookViews>
   <sheets>
     <sheet name="cw.dat" sheetId="1" r:id="rId1"/>
@@ -2153,7 +2153,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6:O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5159,7 +5159,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="O6" sqref="A6:O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8031,2829 +8031,3111 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645F305A-34D8-8541-AEA0-572B2EBD3E45}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3">
         <v>1964</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>1964</v>
+      </c>
+      <c r="B6">
         <v>7.5905199999999997</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>33.050600000000003</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>70.655000000000001</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>61.372599999999998</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>28.0367</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>54.496200000000002</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>24.003299999999999</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>7.4848400000000002</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>4.5957600000000003</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>4.51607</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>4.5083700000000002</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>4.5025899999999996</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>4.4981900000000001</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>4.4933199999999998</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>4.4857699999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
+        <f>A6+1</f>
+        <v>1965</v>
+      </c>
+      <c r="B7">
         <v>21.135999999999999</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>26.016500000000001</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>88.318100000000001</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>232.03299999999999</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>40.088299999999997</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>15.5648</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>28.941299999999998</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>12.638400000000001</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3.96217</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2.44455</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>2.4705599999999999</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>2.4663499999999998</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2.46319</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>2.4607800000000002</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>4.9121100000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
+        <f t="shared" ref="A8:A64" si="0">A7+1</f>
+        <v>1966</v>
+      </c>
+      <c r="B8">
         <v>16.920100000000001</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>92.779899999999998</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>75.433099999999996</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>201.38200000000001</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>125.254</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>21.456800000000001</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>8.48583</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>16.016100000000002</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>7.1024000000000003</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2.26362</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1.45261</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1.4680599999999999</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>1.46556</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>1.4636800000000001</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>4.3811299999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
+        <f t="shared" si="0"/>
+        <v>1967</v>
+      </c>
+      <c r="B9">
         <v>55.681699999999999</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>138.756</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>585.70299999999997</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>209.07499999999999</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>181.06399999999999</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>114.087</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>20.567599999999999</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>8.4472100000000001</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>16.528500000000001</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>7.5865200000000002</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2.4950800000000002</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1.60114</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1.6181700000000001</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>1.6154200000000001</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>6.44245</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
+        <f t="shared" si="0"/>
+        <v>1968</v>
+      </c>
+      <c r="B10">
         <v>67.412800000000004</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>269.45499999999998</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>385.16500000000002</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>641.86099999999999</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>136.65899999999999</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>105.31</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>66.561700000000002</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>11.9129</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>4.8816899999999999</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>9.5475899999999996</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>4.3975600000000004</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1.4462900000000001</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.92810700000000002</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.93798099999999995</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>4.6707799999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
+        <f t="shared" si="0"/>
+        <v>1969</v>
+      </c>
+      <c r="B11">
         <v>109.557</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>254.34299999999999</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>859.72500000000002</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>437.97399999999999</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>340.54500000000002</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>73.576700000000002</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>58.763599999999997</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>38.009599999999999</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>6.9637000000000002</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2.8986999999999998</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>5.7466600000000003</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>2.6468699999999998</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0.87051400000000001</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.55862400000000001</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>3.3758900000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
+        <f t="shared" si="0"/>
+        <v>1970</v>
+      </c>
+      <c r="B12">
         <v>236.4</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>538.69100000000003</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>1024.49</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>742.65800000000002</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>306.90100000000001</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>247.66</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>59.887799999999999</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>50.552199999999999</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>33.416600000000003</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>7.3887</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>3.0758800000000002</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>6.0979000000000001</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>2.8086500000000001</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.92372200000000004</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>4.1749999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
+        <f t="shared" si="0"/>
+        <v>1971</v>
+      </c>
+      <c r="B13">
         <v>224.58500000000001</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>579.18399999999997</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>1298.24</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>796.30200000000002</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>674.46799999999996</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>249.90299999999999</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>200.941</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>47.287500000000001</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>38.558999999999997</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>32.514099999999999</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>5.5160799999999997</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>2.2963100000000001</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>4.5524300000000002</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>2.0968200000000001</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>3.8064800000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
+        <f t="shared" si="0"/>
+        <v>1972</v>
+      </c>
+      <c r="B14">
         <v>129.018</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>557.69600000000003</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>1366.14</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1033.8499999999999</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>537.56700000000001</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>368.41500000000002</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>140.67699999999999</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>123.31100000000001</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>26.7608</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>24.653500000000001</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>13.4434</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>2.2806999999999999</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0.94944099999999998</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>1.88226</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>2.4407999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
+        <f t="shared" si="0"/>
+        <v>1973</v>
+      </c>
+      <c r="B15">
         <v>200.143</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>574.89800000000002</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>867.26300000000003</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>929.77300000000002</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>613.36900000000003</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>320.80799999999999</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>220.79400000000001</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>89.680300000000003</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>70.168400000000005</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>15.7883</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>11.0532</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>6.0272500000000004</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>1.02254</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>0.425676</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>1.93821</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
+        <f t="shared" si="0"/>
+        <v>1974</v>
+      </c>
+      <c r="B16">
         <v>123.474</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>1713.96</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>869.346</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>545.48199999999997</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>442.64</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>283.69099999999997</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>148.79599999999999</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>109.149</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>40.961100000000002</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>31.713100000000001</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>5.98813</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>4.19224</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>2.286</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>0.387824</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.89656999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
+        <f t="shared" si="0"/>
+        <v>1975</v>
+      </c>
+      <c r="B17">
         <v>69.316199999999995</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>770.78300000000002</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>1823.3</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>371.303</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>227.34200000000001</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>181.99700000000001</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>116.474</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>61.524799999999999</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>42.366</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>16.532499999999999</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>12.8362</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>2.4237600000000001</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>1.69685</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>0.92528100000000002</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>0.51987099999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
+        <f t="shared" si="0"/>
+        <v>1976</v>
+      </c>
+      <c r="B18">
         <v>36.909999999999997</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>560.75</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>1296.26</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>755.16800000000001</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>159.91499999999999</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>100.53400000000001</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>81.589699999999993</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>52.508099999999999</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>27.575800000000001</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>18.844799999999999</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>6.6082400000000003</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>5.1307700000000001</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>0.96880100000000002</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>0.67825000000000002</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>0.57764300000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
+        <f t="shared" si="0"/>
+        <v>1977</v>
+      </c>
+      <c r="B19">
         <v>27.4619</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>460.94099999999997</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>909.24300000000005</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>610.678</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>304.89</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>67.280799999999999</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>43.421900000000001</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>35.742600000000003</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>23.1509</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>12.0098</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>7.6881599999999999</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>2.69598</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>2.09321</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>0.39524500000000001</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>0.51236999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
+        <f t="shared" si="0"/>
+        <v>1978</v>
+      </c>
+      <c r="B20">
         <v>36.671300000000002</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>420.41899999999998</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>735.96600000000001</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>612.12400000000002</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>330.25099999999998</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>158.51</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>35.535499999999999</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>23.241900000000001</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>19.819199999999999</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>12.8081</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>6.6033299999999997</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>4.2271799999999997</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>1.4823299999999999</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>1.1509100000000001</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>0.49903399999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
+        <f t="shared" si="0"/>
+        <v>1979</v>
+      </c>
+      <c r="B21">
         <v>68.720500000000001</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>465.92399999999998</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>648.60400000000004</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>409.154</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>348.911</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>181.369</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>88.802400000000006</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>20.149999999999999</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>14.2822</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>11.9649</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>7.7367699999999999</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>3.9887700000000001</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>2.5534500000000002</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>0.89540900000000001</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>0.99665700000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+      <c r="B22">
         <v>15.210800000000001</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>484.50299999999999</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>802.553</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>440.57799999999997</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>256.28800000000001</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>177.66900000000001</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>90.960300000000004</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>45.240400000000001</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>10.6448</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>8.0622500000000006</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>6.5626100000000003</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>4.2435099999999997</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>2.1877900000000001</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>1.4005300000000001</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>1.0377700000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
+        <f t="shared" si="0"/>
+        <v>1981</v>
+      </c>
+      <c r="B23">
         <v>8.1688500000000008</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>96.383700000000005</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>1050.6500000000001</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>658.154</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>233.46199999999999</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>108.455</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>69.844899999999996</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>36.475700000000003</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>19.040700000000001</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>5.5539199999999997</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>3.2910499999999998</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>2.67889</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>1.7322200000000001</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>0.893065</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>0.99532799999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
+        <f t="shared" si="0"/>
+        <v>1982</v>
+      </c>
+      <c r="B24">
         <v>2.17441</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>65.688699999999997</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>183.49100000000001</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>1110.9000000000001</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>375.52</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>96.9221</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>44.918700000000001</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>29.378499999999999</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>16.381900000000002</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>11.7257</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>2.4098199999999999</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>1.42797</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>1.1623600000000001</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>0.75160499999999997</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>0.81936600000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
+        <f t="shared" si="0"/>
+        <v>1983</v>
+      </c>
+      <c r="B25">
         <v>4.8003600000000004</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>50.891199999999998</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>171.4</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>349.52600000000001</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>832.92</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>216.49100000000001</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>55.886499999999998</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>26.3367</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>18.659099999999999</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>14.935499999999999</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>6.8295899999999996</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>1.4035899999999999</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>0.83171799999999996</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.67701199999999995</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>0.91500599999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
+        <f t="shared" si="0"/>
+        <v>1984</v>
+      </c>
+      <c r="B26">
         <v>0.87586399999999998</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>90.354900000000001</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>89.206900000000005</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>369.14400000000001</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>425.25700000000001</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>615.11199999999997</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>132.49600000000001</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>34.564900000000002</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>17.3232</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>16.478999999999999</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>7.6906800000000004</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>3.5167299999999999</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>0.72274499999999997</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>0.42827300000000001</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>0.81977100000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
+        <f t="shared" si="0"/>
+        <v>1985</v>
+      </c>
+      <c r="B27">
         <v>1.8710100000000001</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>29.9163</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>343.97300000000001</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>157.13499999999999</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>366.19600000000003</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>308.87599999999998</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>439.75099999999998</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>96.123599999999996</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>25.280799999999999</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>16.8462</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>9.9978700000000007</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>4.6659600000000001</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>2.13361</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>0.43849199999999999</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>0.757193</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
+        <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+      <c r="B28">
         <v>0.59523899999999996</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>68.554599999999994</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>80.330699999999993</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>625.25800000000004</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>181.102</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>338.59</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>176.75200000000001</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>243.19300000000001</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>60.634700000000002</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>17.7714</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>7.6423800000000002</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>4.5355999999999996</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>2.1167400000000001</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>0.96792699999999998</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>0.54242999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
+        <f t="shared" si="0"/>
+        <v>1987</v>
+      </c>
+      <c r="B29">
         <v>0.193383</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>18.7654</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>151.38999999999999</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>90.571200000000005</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>397.44200000000001</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>119.91800000000001</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>138.02500000000001</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>101.054</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>162.958</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>42.378900000000002</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>10.939500000000001</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>4.7044100000000002</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>2.7919700000000001</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>1.3029999999999999</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>0.92972900000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
+        <f t="shared" si="0"/>
+        <v>1988</v>
+      </c>
+      <c r="B30">
         <v>0.16641800000000001</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>14.130800000000001</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>252.42400000000001</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>405.74099999999999</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>187.58699999999999</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>506.05599999999998</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>138.428</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>152.327</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>76.077399999999997</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>108.468</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>22.011700000000001</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>5.6820300000000001</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>2.4434900000000002</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>1.4501599999999999</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>1.1596900000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
+        <f t="shared" si="0"/>
+        <v>1989</v>
+      </c>
+      <c r="B31">
         <v>0.27977000000000002</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>9.4597899999999999</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>73.8536</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>197.881</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>438.173</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>141.017</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>478.99299999999999</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>91.728800000000007</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>100.756</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>49.418999999999997</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>74.300399999999996</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>15.078099999999999</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>3.8921999999999999</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>1.6737899999999999</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>1.78775</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
+        <f t="shared" si="0"/>
+        <v>1990</v>
+      </c>
+      <c r="B32">
         <v>1.4227099999999999</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>29.7744</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>53.070099999999996</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>199.17</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>331.14299999999997</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>543.75300000000004</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>138.13999999999999</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>370.36900000000003</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>72.148200000000003</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>79.199600000000004</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>39.499400000000001</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>59.386400000000002</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>12.051500000000001</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>3.1109399999999998</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>2.7667199999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
+        <f t="shared" si="0"/>
+        <v>1991</v>
+      </c>
+      <c r="B33">
         <v>0.96194710410000006</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>111.6185583</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>43.471399099999999</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>85.059543599999998</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>156.08907440000002</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>184.518812</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>500.52927500000004</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>76.163121000000004</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>289.23782199999999</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>27.988148690000003</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>139.51794029999999</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>18.327783270000001</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>93.622850900000003</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>23.296670409999997</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>53.556361199999998</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
+        <f t="shared" si="0"/>
+        <v>1992</v>
+      </c>
+      <c r="B34">
         <v>1.09985281</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>84.5847926</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>675.09147800000005</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>129.9378696</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>79.511266300000003</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>108.5632291</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>133.62789309999999</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>253.37719810000002</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>102.1881272</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>146.85471609999999</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>57.897071000000004</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>46.297903910000002</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>13.422353450000001</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>43.780926809999997</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>34.448307800000002</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
+        <f t="shared" si="0"/>
+        <v>1993</v>
+      </c>
+      <c r="B35">
         <v>6.6021388200000003E-2</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>7.4188565280000001</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>260.25280900000001</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>1145.526398</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>102.8740672</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>66.096329400000002</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>66.302082899999988</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>56.410945399999996</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>86.091787400000001</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>21.139141370000001</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>32.649831989999996</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>12.345750019999999</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>13.456079069999999</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>6.7550585250000008</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>16.09871205</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
+        <f t="shared" si="0"/>
+        <v>1994</v>
+      </c>
+      <c r="B36">
         <v>0.74789365200000002</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>30.15340385</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>55.091124700000002</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>360.79458899999997</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>1058.595082</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>175.5192141</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>53.4769997</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>19.085661760000001</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>13.127181670000001</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>20.142310270000003</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>9.7062983040000006</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>9.3720143599999997</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>7.5477257399999997</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>3.9610423130000001</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>8.2887951560000008</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1995</v>
       </c>
       <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
         <v>0.51391798630000007</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>72.826367300000001</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>146.6363341</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>395.07127000000003</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>760.34415300000001</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>136.1404196</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>34.543434150000003</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>12.26048587</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>7.4935222819999998</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>17.45987517</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>4.9984062080000005</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>5.8074557649999994</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>1.655581779</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>8.9111975519999991</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1996</v>
       </c>
       <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
         <v>21.638913349999999</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>48.029722620000001</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>71.707218699999999</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>160.8144704</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>361.54523899999998</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>481.24719900000002</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>184.45250200000001</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>33.60352958</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>13.434920229999999</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>7.9397256159999996</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>8.805008334</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>4.3305731219999997</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>5.8291313630000001</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>5.2985962280000001</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
+        <f t="shared" si="0"/>
+        <v>1997</v>
+      </c>
+      <c r="B39">
         <v>1.0283786370000001</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>77.611102650000007</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>40.28813023</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>118.8646792</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>454.667395</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>288.67107299999998</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>256.12126699999999</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>198.3565859</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>63.955623070000001</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>13.321498020000002</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>5.9638749779999998</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>4.6414892879999998</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>2.891303239</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>4.7764236689999997</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>9.1078412889999996</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
+        <f t="shared" si="0"/>
+        <v>1998</v>
+      </c>
+      <c r="B40">
         <v>0.28780919599999999</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>41.976380340000006</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>84.446906900000002</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>70.424204700000004</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>153.1989873</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>702.10139500000002</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>199.36885699999999</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>131.59447059999999</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>110.63523119999999</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>27.766080720000001</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>6.1388368549999992</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>5.5590458030000001</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>2.5518536649999999</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>2.4991556940000001</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>4.4801357799999995</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
+        <f t="shared" si="0"/>
+        <v>1999</v>
+      </c>
+      <c r="B41">
         <v>0.232155207</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>10.335748130000001</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>298.418049</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>224.808469</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>102.9336656</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>156.86269000000001</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>469.26525600000002</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>130.86590889999999</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>56.445650800000003</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>33.1474154</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>3.9566371600000001</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>2.181584773</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>0.85598967370000001</v>
       </c>
-      <c r="N41">
+      <c r="O41">
         <v>0.47699982299999999</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>2.059401641</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
         <v>16.05972731</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>82.361482999999993</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>428.07334700000001</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>346.165684</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>106.57603230000001</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>168.21673000000001</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>357.35742099999999</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>84.828163499999988</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>29.693388200000001</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>22.021642319999998</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>5.2403648839999999</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>1.4167334009999999</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>0.60805761199999997</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>0.95198711400000002</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2001</v>
       </c>
       <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
         <v>3.2101916299999997</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>42.739398399999999</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>154.34012200000001</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>580.46544499999993</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>414.63521500000002</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>137.04881800000001</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>128.8735441</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>157.07202699999999</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>57.797868100000002</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>33.609301600000002</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>16.189658130000002</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>5.4803057319999997</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>3.0881360739999999</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>1.946522431</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
+        <f t="shared" si="0"/>
+        <v>2002</v>
+      </c>
+      <c r="B44">
         <v>0.77223282900000001</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>46.996577899999998</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>107.93837690000001</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>217.60415</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>287.265333</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>605.72576800000002</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>267.687161</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>98.365051300000005</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>85.798665900000003</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>93.829629799999992</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>34.573591399999998</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>14.387524709999999</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>11.0313517</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>2.9525591209999997</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <v>1.8132781310000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2003</v>
       </c>
       <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
         <v>14.52026993</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>411.35562300000004</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>323.79848599999997</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>360.044668</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>301.17273299999999</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>337.26015999999998</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>158.39455600000002</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>49.369911200000004</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>39.2401366</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>35.6738711</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>22.912768029999999</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>6.6123774099999997</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>3.6413360930000001</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>3.1816738180000002</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2004</v>
       </c>
       <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
         <v>0.53806971580000007</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>89.511192399999999</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>830.28854000000001</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>480.16675500000002</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>236.578172</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>169.11133900000002</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>156.12448999999998</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>64.895669900000001</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>16.101512589999999</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>17.042816200000001</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>25.246428820000002</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <v>9.4379576350000001</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>5.9121913610000005</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <v>6.8654856749999995</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2005</v>
       </c>
       <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
         <v>4.7909620049999999</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>52.0978694</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>392.45952699999998</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>862.93196999999998</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>484.14750300000003</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>159.30457279999999</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>68.014676500000007</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>66.555640799999992</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>30.0704572</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>9.9880773400000002</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>9.1330954079999991</v>
       </c>
-      <c r="M47">
+      <c r="N47">
         <v>3.1905438210000003</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>2.4800766239999996</v>
       </c>
-      <c r="O47">
+      <c r="P47">
         <v>3.4041279720000004</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2006</v>
       </c>
       <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
         <v>9.8835303099999994</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>84.09057709999999</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>295.46819400000004</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>619.00989800000002</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>597.02113399999996</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>278.30899099999999</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>107.2342268</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>47.969024599999997</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>38.327597500000003</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>17.682172040000001</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>8.2328895979999999</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>8.302788542</v>
       </c>
-      <c r="N48">
+      <c r="O48">
         <v>5.315355405</v>
       </c>
-      <c r="O48">
+      <c r="P48">
         <v>7.209422419</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="B49">
         <v>1.65765417</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>15.719014100000001</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>59.123715900000001</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>139.02480110000002</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>389.02224899999999</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>511.47744399999999</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>300.48092200000002</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>136.94723809999999</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>47.559076399999995</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>27.484340599999999</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>21.847872240000001</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>8.9093995900000014</v>
       </c>
-      <c r="M49">
+      <c r="N49">
         <v>6.5241091950000003</v>
       </c>
-      <c r="N49">
+      <c r="O49">
         <v>3.401786779</v>
       </c>
-      <c r="O49">
+      <c r="P49">
         <v>10.780547220000001</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2008</v>
       </c>
       <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
         <v>25.164477999999999</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>58.7608484</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>79.141547900000006</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>146.859691</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>309.36439799999999</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>242.04710399999999</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>148.58482599999999</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>84.191663199999994</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>22.1554401</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>17.548432170000002</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>14.42077681</v>
       </c>
-      <c r="M50">
+      <c r="N50">
         <v>8.6243413600000007</v>
       </c>
-      <c r="N50">
+      <c r="O50">
         <v>2.7666603159999998</v>
       </c>
-      <c r="O50">
+      <c r="P50">
         <v>12.641796560000001</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2009</v>
       </c>
       <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
         <v>1.314498395</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>175.34764300000001</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>200.37920800000001</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>82.471420299999991</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>114.3298441</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>124.19056540000001</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>104.2171651</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>66.572547600000007</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>40.175694700000001</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>23.511255980000001</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>7.6082133670000003</v>
       </c>
-      <c r="M51">
+      <c r="N51">
         <v>7.4586743379999998</v>
       </c>
-      <c r="N51">
+      <c r="O51">
         <v>2.7067472480000001</v>
       </c>
-      <c r="O51">
+      <c r="P51">
         <v>8.7209530290000004</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="B52">
         <v>1.0785094209999999</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>26.428943070000003</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>31.817169440000001</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>558.81399699999997</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>220.26301500000002</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>54.6841674</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>42.964398099999997</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>57.622763400000004</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>51.727377599999997</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>31.7912675</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>15.94892177</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>8.6235509600000011</v>
       </c>
-      <c r="M52">
+      <c r="N52">
         <v>5.9539270770000003</v>
       </c>
-      <c r="N52">
+      <c r="O52">
         <v>4.370871062</v>
       </c>
-      <c r="O52">
+      <c r="P52">
         <v>5.09875305</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="B53">
         <v>0.38119999799999998</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>10.33856984</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>193.13385</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>115.2524401</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>808.35877700000003</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>284.41593499999999</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>63.501076999999995</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>37.475159399999995</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>38.4569081</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>41.370624799999995</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>25.778842870000002</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>12.452666970000001</v>
       </c>
-      <c r="M53">
+      <c r="N53">
         <v>1.7564840529999999</v>
       </c>
-      <c r="N53">
+      <c r="O53">
         <v>3.9715638720000004</v>
       </c>
-      <c r="O53">
+      <c r="P53">
         <v>4.3240444309999999</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2012</v>
       </c>
       <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
         <v>22.24343854</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>116.6276266</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>945.75545700000009</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>172.61298499999998</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>432.12828000000002</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>141.4123792</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>36.643327499999998</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>17.413948000000001</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>14.589028649999999</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>15.90295306</v>
       </c>
-      <c r="L54">
+      <c r="M54">
         <v>13.475815350000001</v>
       </c>
-      <c r="M54">
+      <c r="N54">
         <v>7.3997497789999995</v>
       </c>
-      <c r="N54">
+      <c r="O54">
         <v>6.1355083759999998</v>
       </c>
-      <c r="O54">
+      <c r="P54">
         <v>3.3276886659999998</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="B55">
         <v>1.842478587</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>0.97048942390000004</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>63.881217400000004</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>342.052796</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>954.90987500000006</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>194.237784</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>156.38297560000001</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>69.902266300000008</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>20.657132000000001</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>12.73676515</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>12.742322939999999</v>
       </c>
-      <c r="L55">
+      <c r="M55">
         <v>10.83897387</v>
       </c>
-      <c r="M55">
+      <c r="N55">
         <v>7.8235749119999998</v>
       </c>
-      <c r="N55">
+      <c r="O55">
         <v>4.8002520630000003</v>
       </c>
-      <c r="O55">
+      <c r="P55">
         <v>5.6986998529999999</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2014</v>
       </c>
       <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
         <v>39.180936199999998</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>30.999533189999998</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>167.60898699999998</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>398.89445699999999</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>751.00535600000001</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>210.017011</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>86.143988300000004</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>29.80157616</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>8.9568910150000001</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>4.4856741910000002</v>
       </c>
-      <c r="L56">
+      <c r="M56">
         <v>4.5203580289999996</v>
       </c>
-      <c r="M56">
+      <c r="N56">
         <v>4.5602836559999993</v>
       </c>
-      <c r="N56">
+      <c r="O56">
         <v>2.7612836949999999</v>
       </c>
-      <c r="O56">
+      <c r="P56">
         <v>6.0125002059999995</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2015</v>
       </c>
       <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
         <v>15.45439927</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>631.80913800000008</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>196.20594</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>228.346756</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>383.903099</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>509.62935600000003</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>88.726285500000003</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>42.087676200000004</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>17.634069459999999</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>2.9327011349999998</v>
       </c>
-      <c r="L57">
+      <c r="M57">
         <v>2.0517439030000002</v>
       </c>
-      <c r="M57">
+      <c r="N57">
         <v>3.0913256660000004</v>
       </c>
-      <c r="N57">
+      <c r="O57">
         <v>2.6540513299999997</v>
       </c>
-      <c r="O57">
+      <c r="P57">
         <v>1.2215093019999999</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2016</v>
       </c>
       <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
         <v>0.496855292</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>90.46833629999999</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>1388.9061000000002</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>159.72294200000002</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>174.31859800000001</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>174.6123968</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>224.44967499999998</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>34.043506260000001</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>13.807988380000001</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>7.9874265649999998</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>0.48469008600000002</v>
       </c>
-      <c r="M58">
+      <c r="N58">
         <v>1.1742280809999999</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>0.66830107859999999</v>
       </c>
-      <c r="O58">
+      <c r="P58">
         <v>0.99506335599999995</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2017</v>
       </c>
       <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
         <v>2.1737189239999997</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>28.13910804</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>548.52004199999999</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>898.129728</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>215.27924299999998</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>147.4142229</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>122.0070972</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>97.1532895</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>21.734654210000002</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>7.2062112889999996</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>5.5977045429999999</v>
       </c>
-      <c r="M59">
+      <c r="N59">
         <v>0.49299360599999997</v>
       </c>
-      <c r="N59">
+      <c r="O59">
         <v>0.2446313749</v>
       </c>
-      <c r="O59">
+      <c r="P59">
         <v>0.12621987470000001</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2018</v>
       </c>
       <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
         <v>1.2957518589999999</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>13.78732186</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>114.9042087</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>1214.8864900000001</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>506.060293</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>104.69882249999999</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>81.901005900000001</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>60.563126099999998</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>25.8669133</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>4.2662881539999997</v>
       </c>
-      <c r="L60">
+      <c r="M60">
         <v>1.096769114</v>
       </c>
-      <c r="M60">
+      <c r="N60">
         <v>0.36271430259999998</v>
       </c>
-      <c r="N60">
+      <c r="O60">
         <v>0.63547892699999997</v>
       </c>
-      <c r="O60">
+      <c r="P60">
         <v>0.49500330400000003</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="B61">
         <v>0.69362497699999992</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>10.88745269</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>12.29751336</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>18.344931859999999</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>157.44176800000002</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>915.85017400000004</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>422.03530000000001</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>93.086930800000005</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>52.090309999999995</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>52.936330499999997</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>10.04864867</v>
       </c>
-      <c r="L61">
+      <c r="M61">
         <v>2.9040748079999998</v>
       </c>
-      <c r="M61">
+      <c r="N61">
         <v>0.84206770600000003</v>
       </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
       <c r="O61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="B62">
         <v>3.7288726080000001</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>245.895183</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>85.609421400000002</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>99.166550900000004</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>134.14842540000001</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>548.48801800000001</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>598.28224499999999</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>126.60757520000001</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>53.007337899999996</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>37.834406100000002</v>
       </c>
-      <c r="K62">
+      <c r="L62">
         <v>27.031319230000001</v>
       </c>
-      <c r="L62">
+      <c r="M62">
         <v>6.8941412020000001</v>
       </c>
-      <c r="M62">
+      <c r="N62">
         <v>1.7347607869999999</v>
       </c>
-      <c r="N62">
+      <c r="O62">
         <v>1.168156312</v>
       </c>
-      <c r="O62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2021</v>
       </c>
       <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
         <v>111.34218940000001</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>1295.6568300000001</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>144.0270587</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>109.9548589</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>107.11649180000001</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>309.31857199999996</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>295.75643400000001</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>72.064777899999996</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>26.5193242</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>16.136358519999998</v>
       </c>
-      <c r="L63">
+      <c r="M63">
         <v>8.5006318699999994</v>
       </c>
-      <c r="M63">
+      <c r="N63">
         <v>2.0498387650000001</v>
       </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
       <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
         <v>0.42016624800000002</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="B64">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B64">
+      <c r="C64">
         <v>64.577110000000005</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>174.73101</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>1037.3900100000001</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>182.12301000000002</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>70.819509999999994</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>80.117410000000007</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>139.14301</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>80.71450999999999</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>16.663509999999999</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <v>13.43591</v>
       </c>
-      <c r="L64">
+      <c r="M64">
         <v>4.74688</v>
       </c>
-      <c r="M64">
+      <c r="N64">
         <v>6.7741600000000002</v>
       </c>
-      <c r="N64">
+      <c r="O64">
         <v>1.00736</v>
       </c>
-      <c r="O64">
+      <c r="P64">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A33:O59">
+  <conditionalFormatting sqref="B33:P59">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -42752,7 +43034,7 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:O69"/>
+      <selection activeCell="A6" sqref="A6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45720,8 +46002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA750029-91CE-FD43-8885-6D160A77B335}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45750,7 +46032,7 @@
         <v>1964</v>
       </c>
       <c r="B3">
-        <v>2017</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -50920,8 +51202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F2215C-4C04-9944-9EB2-86902F8C82D6}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A5" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50982,7 +51264,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>1130521.4129999999</v>
@@ -51032,7 +51314,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>451231.99810000003</v>
@@ -51082,7 +51364,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>340017.82789999997</v>
@@ -51132,7 +51414,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>2825074.76</v>
@@ -51182,7 +51464,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>2255748.1140000001</v>
@@ -51232,7 +51514,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>304843.64639999997</v>
@@ -51282,7 +51564,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <v>753772.53300000005</v>
@@ -51332,7 +51614,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>792123.14629999991</v>
@@ -51382,7 +51664,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="B15">
         <v>1713703.095</v>
@@ -51432,7 +51714,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>3101668.5890000002</v>
@@ -51482,7 +51764,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>83</v>
+        <v>1</v>
       </c>
       <c r="B17">
         <v>1394243.936</v>
@@ -51532,7 +51814,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B18">
         <v>1636676.1910000001</v>
@@ -51582,7 +51864,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="B19">
         <v>1091224.523</v>
@@ -51632,7 +51914,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>1464652.746</v>
@@ -51682,7 +51964,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="B21">
         <v>1496622.3130000001</v>
@@ -51732,7 +52014,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>2534849.3119999999</v>
@@ -51782,7 +52064,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="B23">
         <v>660478.03749999998</v>
@@ -51832,7 +52114,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>1064122.4210000001</v>
@@ -51882,7 +52164,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="B25">
         <v>1090205.1710000001</v>
@@ -51932,7 +52214,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>1674765.463</v>
@@ -51982,7 +52264,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <v>760553.82929999998</v>
@@ -52032,7 +52314,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="B28">
         <v>412048.48619999998</v>
@@ -52082,7 +52364,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="B29">
         <v>367366.64110000001</v>
@@ -52132,7 +52414,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="B30">
         <v>383362.39169999998</v>
@@ -52182,7 +52464,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>865769.70070000004</v>
@@ -52232,7 +52514,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="B32">
         <v>2338270.6239999998</v>
@@ -52282,7 +52564,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>505393.21779999998</v>
@@ -52332,7 +52614,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B34">
         <v>792628.24529999995</v>
@@ -52382,7 +52664,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <v>547848.1213</v>
@@ -52432,7 +52714,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="B36">
         <v>1113031.7379999999</v>
@@ -52482,7 +52764,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>117</v>
+        <v>1</v>
       </c>
       <c r="B37">
         <v>1173123.75</v>
@@ -52532,7 +52814,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>121</v>
+        <v>1</v>
       </c>
       <c r="B38">
         <v>1204398.4909999999</v>
@@ -52582,7 +52864,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>137</v>
+        <v>1</v>
       </c>
       <c r="B39">
         <v>2237792.2510000002</v>
@@ -52632,7 +52914,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>152</v>
+        <v>1</v>
       </c>
       <c r="B40">
         <v>1166976.5560000001</v>
@@ -52682,7 +52964,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B41">
         <v>733826.3811</v>
@@ -52732,7 +53014,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B42">
         <v>850143.34039999999</v>
@@ -52782,7 +53064,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B43">
         <v>1027176.711</v>
@@ -52832,7 +53114,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B44">
         <v>2545287.1630000002</v>
@@ -52882,7 +53164,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B45">
         <v>905809.12439999997</v>
@@ -52932,7 +53214,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B46">
         <v>904491.69140000001</v>
@@ -52982,7 +53264,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B47">
         <v>1384453.2609999999</v>

</xml_diff>